<commit_message>
Fixed - export values to CSV rather than expressions
</commit_message>
<xml_diff>
--- a/Results_RandomForest.xlsx
+++ b/Results_RandomForest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="12780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Optimization" sheetId="1" r:id="rId1"/>
@@ -402,11 +402,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="369478200"/>
-        <c:axId val="369477808"/>
+        <c:axId val="160095904"/>
+        <c:axId val="160028800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="369478200"/>
+        <c:axId val="160095904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -525,12 +525,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369477808"/>
+        <c:crossAx val="160028800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="369477808"/>
+        <c:axId val="160028800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369478200"/>
+        <c:crossAx val="160095904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -928,11 +928,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="454308712"/>
-        <c:axId val="454309888"/>
+        <c:axId val="160079256"/>
+        <c:axId val="159911760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="454308712"/>
+        <c:axId val="160079256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="175"/>
@@ -1052,13 +1052,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454309888"/>
+        <c:crossAx val="159911760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="454309888"/>
+        <c:axId val="159911760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454308712"/>
+        <c:crossAx val="160079256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2696,7 +2696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
@@ -10609,8 +10609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12556,7 +12556,7 @@
         <v>340</v>
       </c>
       <c r="B162" s="4" t="str">
-        <f t="shared" ref="B162:B193" si="5">IF(C162,"aml","normal")</f>
+        <f t="shared" ref="B162:B181" si="5">IF(C162,"aml","normal")</f>
         <v>aml</v>
       </c>
       <c r="C162" s="4">

</xml_diff>